<commit_message>
added tabs to record carbon footprint
</commit_message>
<xml_diff>
--- a/_ECF_PETER/facebook_research_act.xlsx
+++ b/_ECF_PETER/facebook_research_act.xlsx
@@ -1,18 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://northeastern-my.sharepoint.com/personal/li_baol_northeastern_edu/Documents/NEU Year 4/Research/carbon footprint/GoodwillResearch/_ECF_PETER/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA6D7D7B-0F13-4D48-B593-4F81EDFC74ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Embodied Carbon (E_CF) Calculat" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="MIT Nodes" sheetId="2" r:id="rId5"/>
+    <sheet name="Embodied Carbon (E_CF) Calculat" sheetId="1" r:id="rId1"/>
+    <sheet name="MIT Nodes" sheetId="2" r:id="rId2"/>
+    <sheet name="Packaging Overhead" sheetId="3" r:id="rId3"/>
+    <sheet name="Embodied Carbon" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
   <si>
     <t># of Integrated Circuits (Nr)</t>
   </si>
@@ -120,39 +142,145 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/List_of_Intel_manufacturing_sites</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>N_r</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>DRAM</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>SoC</t>
+  </si>
+  <si>
+    <t>Part Name</t>
+  </si>
+  <si>
+    <t>Die Area</t>
+  </si>
+  <si>
+    <t>Num of Dies</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>CI_fab (fab carbon intensity)</t>
+  </si>
+  <si>
+    <t>EPA (energy per area)</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>cm^2</t>
+  </si>
+  <si>
+    <t>g CO2 / kWh</t>
+  </si>
+  <si>
+    <t>kWh / cm^2</t>
+  </si>
+  <si>
+    <t>GPA (gas per area)</t>
+  </si>
+  <si>
+    <t>g CO2 / cm^2</t>
+  </si>
+  <si>
+    <t>MPA (raw material per area)</t>
+  </si>
+  <si>
+    <t>Manufacturing Location</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>Gas Abatement</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>E_soc</t>
+  </si>
+  <si>
+    <t>g CO2</t>
+  </si>
+  <si>
+    <t>Memory and Storage</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Carbon-per-size</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>g CO2 / GB</t>
+  </si>
+  <si>
+    <t>K_r (g CO2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -280,104 +408,258 @@
         <bgColor rgb="FFE06666"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="14" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="16" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="17" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="18" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="19" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="20" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="21" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="22" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>15241</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>144615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB360CC9-F414-49F0-B59E-9B1F125FA371}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2453641" y="0"/>
+          <a:ext cx="3032760" cy="647535"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>144615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A09D732-7D0C-4D5D-933A-DBCC96359577}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10439400" y="0"/>
+          <a:ext cx="3032760" cy="647535"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>451579</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{116B010B-5E75-411A-A56A-5F3D1E3177BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10431780" y="723900"/>
+          <a:ext cx="3316699" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>60961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28591</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F68DF6-D6A7-4BC0-8594-9663D2793850}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10439400" y="1569721"/>
+          <a:ext cx="3139440" cy="973470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -567,24 +849,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="21.63"/>
-    <col customWidth="1" min="3" max="3" width="20.63"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -615,10 +902,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="4">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="F2" s="5">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="G2" s="6">
         <v>4.57</v>
@@ -627,37 +914,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="G3" s="6">
         <v>10.32</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="5">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="G4" s="6">
         <v>2.35</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F5" s="5">
         <v>5.6</v>
       </c>
       <c r="G5" s="6">
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F6" s="5">
         <v>6.3</v>
       </c>
@@ -665,7 +952,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F7" s="7">
         <v>6.21</v>
       </c>
@@ -673,7 +960,7 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="7">
         <v>3.948</v>
       </c>
@@ -681,7 +968,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" s="7">
         <v>16.916</v>
       </c>
@@ -689,7 +976,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F10" s="8">
         <v>24.4</v>
       </c>
@@ -697,15 +984,15 @@
         <v>4.09</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F11" s="8">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="G11" s="6">
         <v>3.74</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F12" s="8">
         <v>12.5</v>
       </c>
@@ -713,7 +1000,7 @@
         <v>7.62</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F13" s="8">
         <v>10.7</v>
       </c>
@@ -721,237 +1008,534 @@
         <v>8.86</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" s="4">
-        <v>315.0</v>
+        <v>315</v>
       </c>
       <c r="G14" s="9">
         <v>1.653</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" s="4">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="G15" s="9">
-        <v>1.14</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16" s="4">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="G16" s="9">
-        <v>1.334</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>1.3340000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17" s="4">
-        <v>184.0</v>
+        <v>184</v>
       </c>
       <c r="G17" s="9">
         <v>20.36</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E18" s="4">
-        <v>159.0</v>
+        <v>159</v>
       </c>
       <c r="G18" s="9">
         <v>10.323</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E19" s="4">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="G19" s="9">
-        <v>3.8556</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>3.8555999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E20" s="4">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="G20" s="9">
-        <v>4.747</v>
+        <v>4.7469999999999999</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B1:M14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>704</v>
+      </c>
+      <c r="C2" s="1">
+        <v>32000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>448</v>
+      </c>
+      <c r="E2" s="1">
+        <v>873</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1">
+        <v>224</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1">
+        <v>384</v>
+      </c>
+      <c r="K2" s="1">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1">
+        <v>480</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1">
+        <v>192</v>
+      </c>
+      <c r="K3" s="1">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1">
+        <v>200</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>500</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1">
+        <v>200</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I8" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677D8472-6534-4C07-9407-71A40073A395}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B2:B6)</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2DE9F-1FE4-48E2-B84E-FB6C71B882FD}">
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="18.0"/>
-    <col customWidth="1" min="3" max="3" width="19.63"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" s="1">
-        <v>704.0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>32000.0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>448.0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>873.0</v>
-      </c>
-      <c r="G2" s="13" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1">
-        <v>224.0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="1">
-        <v>384.0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="H3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="G3" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="1">
-        <v>480.0</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="1">
-        <v>192.0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="H5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="1">
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="F8" s="1">
-        <v>500.0</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="F9" s="1">
-        <v>500.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="1" t="s">
-        <v>25</v>
+      <c r="C8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <f>SUM(F9:F11)+SUM(M3:M5)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="I8"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to Embodied Carbon sheet
</commit_message>
<xml_diff>
--- a/_ECF_PETER/facebook_research_act.xlsx
+++ b/_ECF_PETER/facebook_research_act.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://northeastern-my.sharepoint.com/personal/li_baol_northeastern_edu/Documents/NEU Year 4/Research/carbon footprint/GoodwillResearch/_ECF_PETER/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lipet/Downloads/Fall 2022 Classes/GoodwillResearch/_ECF_PETER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA6D7D7B-0F13-4D48-B593-4F81EDFC74ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AC5396-430E-CC43-B3AD-31B5419F2C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2720" yWindow="1260" windowWidth="23260" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Embodied Carbon (E_CF) Calculat" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
   <si>
     <t># of Integrated Circuits (Nr)</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>K_r (g CO2)</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>TSMC</t>
   </si>
 </sst>
 </file>
@@ -428,33 +434,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,13 +871,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,7 +900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -914,7 +920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -925,7 +931,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -936,7 +942,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F5" s="5">
         <v>5.6</v>
       </c>
@@ -944,7 +950,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F6" s="5">
         <v>6.3</v>
       </c>
@@ -952,7 +958,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="7">
         <v>6.21</v>
       </c>
@@ -960,7 +966,7 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="7">
         <v>3.948</v>
       </c>
@@ -968,7 +974,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="7">
         <v>16.916</v>
       </c>
@@ -976,7 +982,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F10" s="8">
         <v>24.4</v>
       </c>
@@ -984,7 +990,7 @@
         <v>4.09</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="8">
         <v>17.899999999999999</v>
       </c>
@@ -992,7 +998,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="8">
         <v>12.5</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>7.62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F13" s="8">
         <v>10.7</v>
       </c>
@@ -1008,7 +1014,7 @@
         <v>8.86</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E14" s="4">
         <v>315</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>1.653</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E15" s="4">
         <v>230</v>
       </c>
@@ -1024,7 +1030,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E16" s="4">
         <v>201</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>1.3340000000000001</v>
       </c>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E17" s="4">
         <v>184</v>
       </c>
@@ -1040,7 +1046,7 @@
         <v>20.36</v>
       </c>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E18" s="4">
         <v>159</v>
       </c>
@@ -1048,7 +1054,7 @@
         <v>10.323</v>
       </c>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E19" s="4">
         <v>48</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>3.8555999999999999</v>
       </c>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E20" s="4">
         <v>65</v>
       </c>
@@ -1076,25 +1082,25 @@
   </sheetPr>
   <dimension ref="B1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="10" t="s">
         <v>12</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="1">
         <v>704</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G3" s="18" t="s">
         <v>26</v>
       </c>
@@ -1187,7 +1193,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" s="19" t="s">
         <v>29</v>
       </c>
@@ -1204,7 +1210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="22" t="s">
         <v>23</v>
       </c>
@@ -1224,7 +1230,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="18" t="s">
         <v>26</v>
       </c>
@@ -1241,7 +1247,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1262,14 +1268,14 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>36</v>
       </c>
@@ -1280,7 +1286,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1296,7 +1302,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1304,7 +1310,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1320,7 +1326,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1342,24 +1348,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2DE9F-1FE4-48E2-B84E-FB6C71B882FD}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>44</v>
       </c>
@@ -1400,7 +1406,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="24" t="s">
         <v>51</v>
       </c>
@@ -1437,40 +1443,82 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <v>380</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>1.2</v>
+      </c>
       <c r="H3">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>380</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>1.2</v>
+      </c>
       <c r="H4">
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
+      <c r="C5">
+        <v>8.15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5">
+        <v>583</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
       <c r="H5">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="24" t="s">
         <v>64</v>
       </c>
@@ -1490,7 +1538,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="24" t="s">
         <v>51</v>
       </c>
@@ -1510,22 +1558,22 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Found the die area, looking for die number
</commit_message>
<xml_diff>
--- a/_ECF_PETER/facebook_research_act.xlsx
+++ b/_ECF_PETER/facebook_research_act.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lipet/Downloads/Fall 2022 Classes/GoodwillResearch/_ECF_PETER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AC5396-430E-CC43-B3AD-31B5419F2C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0764CA87-3C11-1347-B7A0-1CD236A201D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="1260" windowWidth="23260" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8680" yWindow="500" windowWidth="23260" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Embodied Carbon (E_CF) Calculat" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
   <si>
     <t># of Integrated Circuits (Nr)</t>
   </si>
@@ -250,13 +250,19 @@
   </si>
   <si>
     <t>TSMC</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/pdfDocs/second-gen-xeon-scalable-tmsdg-338847-rev001.pdf</t>
+  </si>
+  <si>
+    <t>I found the mechanical drawing for the Platinum and gold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -280,8 +286,15 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,6 +430,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -461,6 +480,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1082,7 +1103,7 @@
   </sheetPr>
   <dimension ref="B1:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1346,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2DE9F-1FE4-48E2-B84E-FB6C71B882FD}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1450,6 +1471,9 @@
       <c r="B3" t="s">
         <v>23</v>
       </c>
+      <c r="C3" s="25">
+        <v>4</v>
+      </c>
       <c r="D3" t="s">
         <v>70</v>
       </c>
@@ -1467,6 +1491,15 @@
       </c>
       <c r="I3">
         <v>200</v>
+      </c>
+      <c r="J3">
+        <v>500</v>
+      </c>
+      <c r="K3">
+        <v>0.875</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
@@ -1476,6 +1509,9 @@
       <c r="B4" t="s">
         <v>26</v>
       </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
       <c r="D4" t="s">
         <v>70</v>
       </c>
@@ -1493,6 +1529,15 @@
       </c>
       <c r="I4">
         <v>200</v>
+      </c>
+      <c r="J4">
+        <v>500</v>
+      </c>
+      <c r="K4">
+        <v>0.875</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
@@ -1514,8 +1559,26 @@
       <c r="F5">
         <v>12</v>
       </c>
+      <c r="G5">
+        <v>1.3374999999999999</v>
+      </c>
       <c r="H5">
         <v>95</v>
+      </c>
+      <c r="I5">
+        <v>220</v>
+      </c>
+      <c r="J5">
+        <v>500</v>
+      </c>
+      <c r="K5">
+        <v>0.875</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>13969.216</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
@@ -1579,7 +1642,17 @@
       </c>
       <c r="B13">
         <f>SUM(F9:F11)+SUM(M3:M5)</f>
-        <v>0</v>
+        <v>13969.216</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C19" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C20" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Nov 21, 2022
</commit_message>
<xml_diff>
--- a/_ECF_PETER/facebook_research_act.xlsx
+++ b/_ECF_PETER/facebook_research_act.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lipet/Downloads/Fall 2022 Classes/GoodwillResearch/_ECF_PETER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E36EA15-FA7D-0944-90C2-CB83E880BE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D10EF74-FC54-5447-B588-95F92D92EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="5960" windowWidth="24760" windowHeight="16240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4040" yWindow="3540" windowWidth="24760" windowHeight="16240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Embodied Carbon (E_CF) Calculat" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
   <si>
     <t># of Integrated Circuits (Nr)</t>
   </si>
@@ -252,7 +252,22 @@
     <t>TSMC</t>
   </si>
   <si>
-    <t>This is not anywhere?</t>
+    <t>https://web.archive.org/web/20160706231128/http://ddr4.org/contact-us</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Samsung-PC4-21300-2666MHZ-desktop-memory/dp/B07F72RJYN</t>
+  </si>
+  <si>
+    <t>870 EVO SATA 2.5" SSD 4 TB</t>
+  </si>
+  <si>
+    <t>Samsung 8GB DDR4 PC4-21300</t>
+  </si>
+  <si>
+    <t>https://www.westerndigital.com/products/internal-drives/wd-blue-sata-2-5-ssd?ef_id=Cj0KCQiA4OybBhCzARIsAIcfn9masMsJLktL8OgSPeaWW9fMF_CxrXgOa-NTl5dSaxyt1OiJoF7ZqRcaAirvEALw_wcB:G:s&amp;s_kwcid=AL!15012!3!!!!x!!!17824513874!&amp;utm_medium=pdsh2&amp;utm_source=gads&amp;utm_campaign=WD-NA-US-PLA&amp;utm_content=&amp;utm_term=WDS400T2B0A#WDS400T2B0A</t>
+  </si>
+  <si>
+    <t># of Parts</t>
   </si>
 </sst>
 </file>
@@ -559,13 +574,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>175260</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>144615</xdr:rowOff>
@@ -603,13 +618,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>451579</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -647,13 +662,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>60961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>28591</xdr:rowOff>
@@ -1293,7 +1308,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1374,26 +1389,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2DE9F-1FE4-48E2-B84E-FB6C71B882FD}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>44</v>
       </c>
@@ -1401,200 +1417,204 @@
         <v>45</v>
       </c>
       <c r="C1" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="L1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="24" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="E2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>56</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="24"/>
+      <c r="K2" s="24" t="s">
+        <v>56</v>
+      </c>
       <c r="L2" s="24"/>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="24"/>
+      <c r="N2" s="24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="25">
+      <c r="D3" s="25">
         <v>6.94</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>70</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>380</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>14</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1.2</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>95</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>200</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>500</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.875</v>
       </c>
-      <c r="L3" s="25">
+      <c r="M3" s="25">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>9168.73</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>6.94</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>70</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>380</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>14</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.2</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>95</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>200</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>500</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.875</v>
       </c>
-      <c r="L4" s="25">
+      <c r="M4" s="25">
         <v>1</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>9168.73</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>8.15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>71</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>583</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>12</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1.3374999999999999</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>95</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>220</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>500</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.875</v>
       </c>
-      <c r="L5" s="25">
+      <c r="M5" s="25">
         <v>1</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>13969.216</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="24" t="s">
         <v>64</v>
       </c>
@@ -1602,73 +1622,110 @@
         <v>45</v>
       </c>
       <c r="C7" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="E7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="F7" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="G7" s="24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="24" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="E8" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="F8" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="G8" s="24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>65</v>
+      </c>
+      <c r="G9">
+        <v>520</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <v>4000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>10.7</v>
+      </c>
+      <c r="G10">
+        <v>42800</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13">
-        <f>SUM(F9:F11)+SUM(M3:M5)</f>
-        <v>32306.675999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C19" s="26"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C20" s="27"/>
+        <f>SUM(G9:G11)+SUM(N3:N5)</f>
+        <v>75626.676000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D19" s="26"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D20" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update excel file with N_r
</commit_message>
<xml_diff>
--- a/_ECF_PETER/facebook_research_act.xlsx
+++ b/_ECF_PETER/facebook_research_act.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baoli\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lipet/Downloads/Fall 2022 Classes/GoodwillResearch/_ECF_PETER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0417BEEC-337E-42C6-ABE7-27537932AE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2240888E-CD6A-9D42-A498-470E60428A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28780" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Embodied Carbon (E_CF) Calculat" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t># of Integrated Circuits (Nr)</t>
   </si>
@@ -270,10 +270,10 @@
     <t># of Parts</t>
   </si>
   <si>
-    <t>DRAM (CPU)</t>
-  </si>
-  <si>
-    <t>DRAM (GPU)</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nvidia Volta V100 </t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -509,6 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,13 +532,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>15241</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>144615</xdr:rowOff>
@@ -670,13 +671,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>60961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>28591</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -716,42 +717,42 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Grayscale">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="F8F8F8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="DDDDDD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="B2B2B2"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="969696"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="808080"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="5F5F5F"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="4D4D4D"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="5F5F5F"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="919191"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
@@ -920,13 +921,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,7 +950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -969,7 +970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -980,7 +981,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -991,7 +992,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F5" s="5">
         <v>5.6</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F6" s="5">
         <v>6.3</v>
       </c>
@@ -1007,7 +1008,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="7">
         <v>6.21</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="7">
         <v>3.948</v>
       </c>
@@ -1023,7 +1024,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="7">
         <v>16.916</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F10" s="8">
         <v>24.4</v>
       </c>
@@ -1039,7 +1040,7 @@
         <v>4.09</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="8">
         <v>17.899999999999999</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="8">
         <v>12.5</v>
       </c>
@@ -1055,7 +1056,7 @@
         <v>7.62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F13" s="8">
         <v>10.7</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>8.86</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E14" s="4">
         <v>315</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>1.653</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E15" s="4">
         <v>230</v>
       </c>
@@ -1079,7 +1080,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E16" s="4">
         <v>201</v>
       </c>
@@ -1087,7 +1088,7 @@
         <v>1.3340000000000001</v>
       </c>
     </row>
-    <row r="17" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E17" s="4">
         <v>184</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>20.36</v>
       </c>
     </row>
-    <row r="18" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E18" s="4">
         <v>159</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>10.323</v>
       </c>
     </row>
-    <row r="19" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E19" s="4">
         <v>48</v>
       </c>
@@ -1111,7 +1112,7 @@
         <v>3.8555999999999999</v>
       </c>
     </row>
-    <row r="20" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E20" s="4">
         <v>65</v>
       </c>
@@ -1135,21 +1136,21 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="10" t="s">
         <v>12</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="1">
         <v>704</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G3" s="18" t="s">
         <v>26</v>
       </c>
@@ -1242,7 +1243,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" s="19" t="s">
         <v>29</v>
       </c>
@@ -1259,7 +1260,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="22" t="s">
         <v>23</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="18" t="s">
         <v>26</v>
       </c>
@@ -1296,7 +1297,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1311,79 +1312,121 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677D8472-6534-4C07-9407-71A40073A395}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="24" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C2">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="28">
+        <v>16</v>
+      </c>
+      <c r="D2" s="28">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="C3">
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4">
+        <v>26</v>
+      </c>
+      <c r="D4">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="C4">
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>41</v>
       </c>
-      <c r="C5">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>42</v>
       </c>
-      <c r="C6">
+      <c r="D7">
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B7">
-        <f>SUM(B2:B6)</f>
-        <v>0</v>
-      </c>
-      <c r="C7">
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>60</v>
+      </c>
+      <c r="D8">
         <v>150</v>
       </c>
     </row>
@@ -1397,26 +1440,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2DE9F-1FE4-48E2-B84E-FB6C71B882FD}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>44</v>
       </c>
@@ -1460,7 +1502,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="24" t="s">
         <v>51</v>
       </c>
@@ -1498,7 +1540,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1539,7 +1581,7 @@
         <v>9168.73</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1580,7 +1622,7 @@
         <v>9168.73</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1621,7 +1663,7 @@
         <v>13969.216</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="24" t="s">
         <v>64</v>
       </c>
@@ -1644,7 +1686,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="24" t="s">
         <v>51</v>
       </c>
@@ -1665,82 +1707,89 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>65</v>
+      </c>
+      <c r="G9">
+        <v>520</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
+        <v>4000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
       </c>
       <c r="F10">
-        <v>65</v>
+        <v>10.7</v>
       </c>
       <c r="G10">
-        <v>520</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>42800</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11">
-        <v>4000</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11">
-        <v>10.7</v>
-      </c>
-      <c r="G11">
-        <v>42800</v>
-      </c>
-      <c r="H11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>43</v>
       </c>
       <c r="B14">
-        <f>SUM(G10:G12)+SUM(N3:N5)</f>
+        <f>SUM(G9:G11)+SUM(N3:N5)</f>
         <v>75626.676000000007</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D20" s="26"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D21" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>